<commit_message>
links extraction issue fixed
</commit_message>
<xml_diff>
--- a/Input/Deal_Date_Input.xlsx
+++ b/Input/Deal_Date_Input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Preqin Deal Date Process\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Damco RPA Projects\Preqin DealDate Process\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Combinations" sheetId="4" r:id="rId1"/>
@@ -6694,9 +6694,9 @@
   </sheetPr>
   <dimension ref="A1:E1545"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -25675,211 +25675,214 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:A43"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>2017</v>
+      </c>
+    </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
-        <v>2055</v>
+      <c r="A4" s="3" t="s">
+        <v>2018</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>2022</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="3" t="s">
-        <v>2023</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>2024</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="3" t="s">
-        <v>2025</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
-        <v>2026</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="3" t="s">
-        <v>2027</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
-        <v>2028</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="3" t="s">
-        <v>2029</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="3" t="s">
-        <v>2030</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
-        <v>2031</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="3" t="s">
-        <v>2032</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="3" t="s">
-        <v>2033</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="3" t="s">
-        <v>2034</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
-        <v>2035</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="3" t="s">
-        <v>2036</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="3" t="s">
-        <v>2037</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
-        <v>2038</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
-        <v>2039</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="3" t="s">
-        <v>2040</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="3" t="s">
-        <v>2041</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="3" t="s">
-        <v>2042</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="3" t="s">
-        <v>2043</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="3" t="s">
-        <v>2044</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
-        <v>2045</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="3" t="s">
-        <v>2046</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">
-        <v>2047</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="3" t="s">
-        <v>2048</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="3" t="s">
-        <v>2049</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="3" t="s">
-        <v>2050</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3" t="s">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3" t="s">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3" t="s">
         <v>2054</v>
       </c>
     </row>

</xml_diff>